<commit_message>
creation of component categories and species risk distribution plots. improvement of other plots. fix LMM and do post hoc tests
</commit_message>
<xml_diff>
--- a/data/black_grass_info/Farmer Focus strategies_01-03-2021.xlsx
+++ b/data/black_grass_info/Farmer Focus strategies_01-03-2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/black_grass_info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/project_git_repo/data/black_grass_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EBFBB3-0F74-A345-A018-C8C3845D2839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7208C9E1-6AAB-B148-BF37-3709E3B42033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{21FD6D02-D7F6-4092-AEE3-1D30A3DBE076}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{21FD6D02-D7F6-4092-AEE3-1D30A3DBE076}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="9" r:id="rId1"/>
@@ -14362,7 +14362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E86CC1-AD7F-496F-A4D4-B1EE54CB89E2}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
@@ -17482,8 +17482,8 @@
   </sheetPr>
   <dimension ref="B1:S62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
minor changes to graphs for presentation
</commit_message>
<xml_diff>
--- a/data/black_grass_info/Farmer Focus strategies_01-03-2021.xlsx
+++ b/data/black_grass_info/Farmer Focus strategies_01-03-2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/project_git_repo/data/black_grass_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7208C9E1-6AAB-B148-BF37-3709E3B42033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0FF4D3-93C6-2249-B924-FA6C90BFBE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{21FD6D02-D7F6-4092-AEE3-1D30A3DBE076}"/>
   </bookViews>
@@ -17482,8 +17482,8 @@
   </sheetPr>
   <dimension ref="B1:S62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>